<commit_message>
Added freeipa.md and update disx-xfs.txt
</commit_message>
<xml_diff>
--- a/disks-partitioning.xlsx
+++ b/disks-partitioning.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t xml:space="preserve">80 GiB VM</t>
   </si>
   <si>
     <t xml:space="preserve">20 GiB VM, 16GB RAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FREEIPA, 16GB RAM</t>
   </si>
   <si>
     <t xml:space="preserve">/boot/eft</t>
@@ -187,8 +190,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -209,204 +216,247 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="0" t="s">
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="0" t="n">
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="n">
         <v>0.6</v>
       </c>
+      <c r="E2" s="1" t="n">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="E3" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>8</v>
+      <c r="A4" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>9</v>
+      <c r="A6" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="0" t="n">
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="n">
         <v>2.4</v>
       </c>
+      <c r="E9" s="1" t="n">
+        <v>2.4</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="D14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="1" t="n">
+        <f aca="false">SUM(D2:D16)</f>
         <v>20</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="0" t="n">
-        <f aca="false">SUM(D2:D16)</f>
+      <c r="E18" s="1" t="n">
+        <f aca="false">SUM(E2:E16)</f>
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Debian, Disk & KVM/QEMU files
</commit_message>
<xml_diff>
--- a/disks-partitioning.xlsx
+++ b/disks-partitioning.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="69">
   <si>
     <t xml:space="preserve">80 GiB VM</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">FREEIPA, 16GB RAM</t>
   </si>
   <si>
-    <t xml:space="preserve">/boot/eft</t>
+    <t xml:space="preserve">/boot/efi</t>
   </si>
   <si>
     <t xml:space="preserve">VFAT (fat32)</t>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">ext2,ext4,xfs</t>
   </si>
   <si>
-    <t xml:space="preserve">1024 GiB</t>
+    <t xml:space="preserve">1024 Mb</t>
   </si>
   <si>
     <t xml:space="preserve">bootbios</t>
@@ -55,7 +55,40 @@
     <t xml:space="preserve">3 Volumes ( One LVM for all below)</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;swap&gt;</t>
+    <t xml:space="preserve">/tmp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">etx4,XFS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-16Gb (10-16 Recommended)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 to LARGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 to 200Gb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/var</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 LARGE for VM’s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/usr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10-100Gb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[SWAP]</t>
   </si>
   <si>
     <t xml:space="preserve">ZRAM optional</t>
@@ -64,31 +97,10 @@
     <t xml:space="preserve">4 for 16Gb RAM, 8 for 32Gb RAM, 16 for 64GB RAM, 32 for 128Gb RAM</t>
   </si>
   <si>
-    <t xml:space="preserve">/tmp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">etx4,XFS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-16Gb (10-16 Recommended)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 to LARGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 to 200Gb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/var</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 LARGE for VM’s</t>
+    <t xml:space="preserve">FREE SPACE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES</t>
   </si>
   <si>
     <t xml:space="preserve">/var/log</t>
@@ -106,16 +118,115 @@
     <t xml:space="preserve">*** /etc</t>
   </si>
   <si>
-    <t xml:space="preserve">/usr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10-100Gb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FREE SPACE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YES</t>
+    <t xml:space="preserve">Directory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Essential command binaries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Static files of the boot loader</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Device files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">etc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Host-specific system configuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User home directories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Essential shared libraries and kernel modules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contains mount points for replaceable media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mount point for mounting a file system temporarily</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virtual directory for system information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">root</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home directory for the root user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run-time variable data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sbin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Essential system binaries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tmp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temporary files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">usr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secondary hierarchy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">var</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variable data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">srv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data for services provided by the system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add-on application software packages</t>
   </si>
 </sst>
 </file>
@@ -125,7 +236,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -147,13 +258,26 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -190,12 +314,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -208,6 +348,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -216,10 +416,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -284,31 +484,18 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>4</v>
-      </c>
+      <c r="A7" s="0"/>
+      <c r="B7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>2</v>
@@ -319,13 +506,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>2.4</v>
@@ -336,13 +523,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>2</v>
@@ -353,113 +540,285 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="1" t="n">
+      <c r="D17" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E17" s="2" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E15" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E16" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="1" t="n">
-        <f aca="false">SUM(D2:D16)</f>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D19" s="1" t="n">
+        <f aca="false">SUM(D2:D17)</f>
         <v>20</v>
       </c>
-      <c r="E18" s="1" t="n">
-        <f aca="false">SUM(E2:E16)</f>
+      <c r="E19" s="1" t="n">
+        <f aca="false">SUM(E2:E17)</f>
         <v>20</v>
       </c>
     </row>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add proxmox.txt and Update disks.txt
</commit_message>
<xml_diff>
--- a/disks-partitioning.xlsx
+++ b/disks-partitioning.xlsx
@@ -418,14 +418,15 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="64.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -482,10 +483,6 @@
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0"/>
-      <c r="B7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">

</xml_diff>

<commit_message>
ADD SSH SHA-256 SHOW
</commit_message>
<xml_diff>
--- a/disks-partitioning.xlsx
+++ b/disks-partitioning.xlsx
@@ -79,13 +79,13 @@
     <t xml:space="preserve">/var</t>
   </si>
   <si>
-    <t xml:space="preserve">20 LARGE for VM’s</t>
+    <t xml:space="preserve">20 to LARGE for VM’s</t>
   </si>
   <si>
     <t xml:space="preserve">/usr</t>
   </si>
   <si>
-    <t xml:space="preserve">10-100Gb</t>
+    <t xml:space="preserve">10-100Gb or LARGE</t>
   </si>
   <si>
     <t xml:space="preserve">[SWAP]</t>
@@ -106,7 +106,7 @@
     <t xml:space="preserve">/var/log</t>
   </si>
   <si>
-    <t xml:space="preserve">LARGE is faving logs</t>
+    <t xml:space="preserve">LARGE is for saving LARGE logs</t>
   </si>
   <si>
     <t xml:space="preserve">/var/lib/libvirt/images</t>
@@ -419,14 +419,16 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="64.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="64.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.19"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Modified disk partitioning, nvme and added
</commit_message>
<xml_diff>
--- a/disks-partitioning.xlsx
+++ b/disks-partitioning.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="70">
   <si>
     <t xml:space="preserve">80 GiB VM</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t xml:space="preserve">ext2,ext4,xfs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bootbios</t>
   </si>
   <si>
     <t xml:space="preserve">/</t>
@@ -427,6 +424,112 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -435,10 +538,10 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.4"/>
@@ -513,26 +616,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>60</v>
@@ -541,90 +662,90 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>60</v>
+        <v>400</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>60</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>400</v>
+        <v>20</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>400</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F9" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>2</v>
-      </c>
       <c r="E10" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>16</v>
@@ -633,58 +754,52 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="46.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="D11" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>16</v>
+        <v>200</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>100</v>
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D14" s="3" t="n">
         <v>0</v>
@@ -695,13 +810,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D15" s="3" t="n">
         <v>0</v>
@@ -710,146 +825,137 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="4" t="s">
+      <c r="D17" s="1" t="n">
+        <f aca="false">SUM(D2:D15)</f>
+        <v>20</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <f aca="false">SUM(E2:E15)</f>
+        <v>20</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <f aca="false">SUM(F2:F16)</f>
+        <v>776</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <f aca="false">SUM(G2:G16)</f>
+        <v>674</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="1" t="n">
-        <f aca="false">SUM(D2:D16)</f>
-        <v>20</v>
-      </c>
-      <c r="E18" s="1" t="n">
-        <f aca="false">SUM(E2:E16)</f>
-        <v>20</v>
-      </c>
-      <c r="F18" s="1" t="n">
-        <f aca="false">SUM(F2:F17)</f>
-        <v>776</v>
-      </c>
-      <c r="G18" s="1" t="n">
-        <f aca="false">SUM(G2:G17)</f>
-        <v>674</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
+      <c r="B18" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="5" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
         <v>35</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -857,49 +963,42 @@
         <v>60</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>